<commit_message>
Encore des chgmts de titres
</commit_message>
<xml_diff>
--- a/Data/EUDA/Cannabis_detaille/a_la_demande_de_deja_traite.xlsx
+++ b/Data/EUDA/Cannabis_detaille/a_la_demande_de_deja_traite.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,52 +441,47 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Year of Treatment</t>
+          <t>Court / probation / police.deja.deja.deja</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Court / probation / police</t>
+          <t>General practitioner.deja.deja.deja</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>General practitioner</t>
+          <t>Other drug treatment centre.deja.deja.deja</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Other drug treatment centre</t>
+          <t>Other health, medical or social service.deja.deja.deja</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Other health, medical or social service</t>
+          <t>Educational services.deja.deja.deja</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Educational services</t>
+          <t>Self-referral, referral from family, friends, etc.; no other agency/institution involved.deja.deja.deja</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Self-referral, referral from family, friends, etc.; no other agency/institution involved</t>
+          <t>Other.deja.deja.deja</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Not known / missing.deja.deja.deja</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Not known / missing</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
+          <t>Total.deja.deja.deja</t>
         </is>
       </c>
     </row>
@@ -497,33 +492,30 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2022</v>
+        <v>158</v>
       </c>
       <c r="C2" t="n">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E2" t="n">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="F2" t="n">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="H2" t="n">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="I2" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="J2" t="n">
-        <v>26</v>
-      </c>
-      <c r="K2" t="n">
         <v>458</v>
       </c>
     </row>
@@ -534,33 +526,30 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2022</v>
+        <v>378</v>
       </c>
       <c r="C3" t="n">
-        <v>378</v>
+        <v>60</v>
       </c>
       <c r="D3" t="n">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E3" t="n">
-        <v>57</v>
+        <v>249</v>
       </c>
       <c r="F3" t="n">
-        <v>249</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>654</v>
       </c>
       <c r="H3" t="n">
-        <v>654</v>
+        <v>19</v>
       </c>
       <c r="I3" t="n">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="J3" t="n">
-        <v>107</v>
-      </c>
-      <c r="K3" t="n">
         <v>1524</v>
       </c>
     </row>
@@ -571,33 +560,30 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2022</v>
+        <v>16</v>
       </c>
       <c r="C4" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="n">
-        <v>2</v>
-      </c>
       <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>21</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>1</v>
       </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>21</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
       <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
         <v>42</v>
       </c>
     </row>
@@ -608,31 +594,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2022</v>
+        <v>51</v>
       </c>
       <c r="C5" t="n">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
         <v>28</v>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>81</v>
+      </c>
       <c r="H5" t="n">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="I5" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" t="n">
-        <v>10</v>
-      </c>
-      <c r="K5" t="n">
         <v>190</v>
       </c>
     </row>
@@ -643,33 +626,30 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2022</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H6" t="n">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="I6" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" t="n">
         <v>66</v>
       </c>
     </row>
@@ -680,33 +660,30 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2020</v>
+        <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D7" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E7" t="n">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="F7" t="n">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>250</v>
       </c>
       <c r="H7" t="n">
-        <v>250</v>
+        <v>4</v>
       </c>
       <c r="I7" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="J7" t="n">
-        <v>24</v>
-      </c>
-      <c r="K7" t="n">
         <v>469</v>
       </c>
     </row>
@@ -717,33 +694,30 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2022</v>
+        <v>94</v>
       </c>
       <c r="C8" t="n">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E8" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="F8" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="G8" t="n">
-        <v>12</v>
+        <v>1148</v>
       </c>
       <c r="H8" t="n">
-        <v>1148</v>
+        <v>130</v>
       </c>
       <c r="I8" t="n">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="J8" t="n">
-        <v>9</v>
-      </c>
-      <c r="K8" t="n">
         <v>1473</v>
       </c>
     </row>
@@ -753,22 +727,19 @@
           <t>Estonia</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>2022</v>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
+      <c r="D9" t="n">
         <v>1</v>
       </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
+      <c r="G9" t="n">
         <v>14</v>
       </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="n">
+      <c r="J9" t="n">
         <v>15</v>
       </c>
     </row>
@@ -779,33 +750,30 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2021</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>7</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>13</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
         <v>3</v>
       </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>7</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>13</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
       <c r="J10" t="n">
-        <v>3</v>
-      </c>
-      <c r="K10" t="n">
         <v>26</v>
       </c>
     </row>
@@ -816,33 +784,30 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2020</v>
+        <v>2482</v>
       </c>
       <c r="C11" t="n">
-        <v>2482</v>
+        <v>215</v>
       </c>
       <c r="D11" t="n">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="E11" t="n">
-        <v>188</v>
+        <v>608</v>
       </c>
       <c r="F11" t="n">
-        <v>608</v>
+        <v>95</v>
       </c>
       <c r="G11" t="n">
-        <v>95</v>
+        <v>2422</v>
       </c>
       <c r="H11" t="n">
-        <v>2422</v>
+        <v>77</v>
       </c>
       <c r="I11" t="n">
-        <v>77</v>
+        <v>764</v>
       </c>
       <c r="J11" t="n">
-        <v>764</v>
-      </c>
-      <c r="K11" t="n">
         <v>6851</v>
       </c>
     </row>
@@ -853,33 +818,30 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2022</v>
+        <v>1510</v>
       </c>
       <c r="C12" t="n">
-        <v>1510</v>
+        <v>62</v>
       </c>
       <c r="D12" t="n">
+        <v>311</v>
+      </c>
+      <c r="E12" t="n">
+        <v>722</v>
+      </c>
+      <c r="F12" t="n">
         <v>62</v>
       </c>
-      <c r="E12" t="n">
-        <v>311</v>
-      </c>
-      <c r="F12" t="n">
-        <v>722</v>
-      </c>
       <c r="G12" t="n">
-        <v>62</v>
+        <v>3773</v>
       </c>
       <c r="H12" t="n">
-        <v>3773</v>
+        <v>260</v>
       </c>
       <c r="I12" t="n">
-        <v>260</v>
+        <v>221</v>
       </c>
       <c r="J12" t="n">
-        <v>221</v>
-      </c>
-      <c r="K12" t="n">
         <v>6921</v>
       </c>
     </row>
@@ -890,33 +852,30 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2022</v>
+        <v>18</v>
       </c>
       <c r="C13" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D13" t="n">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="E13" t="n">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
+        <v>199</v>
+      </c>
+      <c r="H13" t="n">
+        <v>19</v>
+      </c>
+      <c r="I13" t="n">
         <v>1</v>
       </c>
-      <c r="H13" t="n">
-        <v>199</v>
-      </c>
-      <c r="I13" t="n">
-        <v>19</v>
-      </c>
       <c r="J13" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" t="n">
         <v>299</v>
       </c>
     </row>
@@ -927,33 +886,30 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2022</v>
+        <v>359</v>
       </c>
       <c r="C14" t="n">
-        <v>359</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" t="n">
+        <v>25</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>85</v>
+      </c>
+      <c r="H14" t="n">
+        <v>14</v>
+      </c>
+      <c r="I14" t="n">
         <v>1</v>
       </c>
-      <c r="E14" t="n">
-        <v>3</v>
-      </c>
-      <c r="F14" t="n">
-        <v>25</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>85</v>
-      </c>
-      <c r="I14" t="n">
-        <v>14</v>
-      </c>
       <c r="J14" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" t="n">
         <v>488</v>
       </c>
     </row>
@@ -964,33 +920,30 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2022</v>
+        <v>80</v>
       </c>
       <c r="C15" t="n">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="D15" t="n">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="E15" t="n">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="F15" t="n">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="G15" t="n">
-        <v>11</v>
+        <v>353</v>
       </c>
       <c r="H15" t="n">
-        <v>353</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15" t="n">
-        <v>2</v>
-      </c>
-      <c r="K15" t="n">
         <v>650</v>
       </c>
     </row>
@@ -1001,33 +954,30 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2022</v>
+        <v>461</v>
       </c>
       <c r="C16" t="n">
-        <v>461</v>
+        <v>32</v>
       </c>
       <c r="D16" t="n">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="E16" t="n">
-        <v>104</v>
+        <v>312</v>
       </c>
       <c r="F16" t="n">
-        <v>312</v>
+        <v>7</v>
       </c>
       <c r="G16" t="n">
-        <v>7</v>
+        <v>1291</v>
       </c>
       <c r="H16" t="n">
-        <v>1291</v>
+        <v>1092</v>
       </c>
       <c r="I16" t="n">
-        <v>1092</v>
+        <v>23</v>
       </c>
       <c r="J16" t="n">
-        <v>23</v>
-      </c>
-      <c r="K16" t="n">
         <v>3322</v>
       </c>
     </row>
@@ -1038,33 +988,30 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2022</v>
+        <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F17" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="H17" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" t="n">
-        <v>2</v>
-      </c>
-      <c r="K17" t="n">
         <v>76</v>
       </c>
     </row>
@@ -1075,27 +1022,24 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C18" t="n">
-        <v>2</v>
-      </c>
-      <c r="D18" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
       <c r="E18" t="n">
-        <v>2</v>
-      </c>
-      <c r="F18" t="n">
         <v>1</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>4</v>
+      </c>
       <c r="H18" t="n">
-        <v>4</v>
-      </c>
-      <c r="I18" t="n">
-        <v>2</v>
-      </c>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="n">
         <v>11</v>
       </c>
     </row>
@@ -1106,31 +1050,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C19" t="n">
         <v>15</v>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="H19" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
         <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
-      </c>
-      <c r="K19" t="n">
         <v>51</v>
       </c>
     </row>
@@ -1141,31 +1082,28 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2022</v>
+        <v>22</v>
       </c>
       <c r="C20" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
-      </c>
-      <c r="F20" t="n">
         <v>39</v>
       </c>
-      <c r="G20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>68</v>
+      </c>
       <c r="H20" t="n">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="I20" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="J20" t="n">
-        <v>4</v>
-      </c>
-      <c r="K20" t="n">
         <v>151</v>
       </c>
     </row>
@@ -1176,33 +1114,30 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2015</v>
+        <v>24</v>
       </c>
       <c r="C21" t="n">
-        <v>24</v>
+        <v>575</v>
       </c>
       <c r="D21" t="n">
-        <v>575</v>
+        <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="F21" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="H21" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I21" t="n">
-        <v>20</v>
+        <v>861</v>
       </c>
       <c r="J21" t="n">
-        <v>861</v>
-      </c>
-      <c r="K21" t="n">
         <v>1577</v>
       </c>
     </row>
@@ -1212,22 +1147,19 @@
           <t>Norway</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>2022</v>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>737</v>
+      </c>
       <c r="J22" t="n">
         <v>737</v>
       </c>
-      <c r="K22" t="n">
-        <v>737</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1236,33 +1168,30 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2022</v>
+        <v>17</v>
       </c>
       <c r="C23" t="n">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="D23" t="n">
-        <v>139</v>
+        <v>59</v>
       </c>
       <c r="E23" t="n">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="F23" t="n">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="G23" t="n">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="H23" t="n">
-        <v>159</v>
+        <v>21</v>
       </c>
       <c r="I23" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="J23" t="n">
-        <v>2</v>
-      </c>
-      <c r="K23" t="n">
         <v>490</v>
       </c>
     </row>
@@ -1273,31 +1202,28 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2022</v>
+        <v>155</v>
       </c>
       <c r="C24" t="n">
-        <v>155</v>
+        <v>14</v>
       </c>
       <c r="D24" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E24" t="n">
+        <v>54</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>99</v>
+      </c>
+      <c r="H24" t="n">
+        <v>12</v>
+      </c>
+      <c r="I24" t="n">
         <v>4</v>
       </c>
-      <c r="F24" t="n">
-        <v>54</v>
-      </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="n">
-        <v>99</v>
-      </c>
-      <c r="I24" t="n">
-        <v>12</v>
-      </c>
       <c r="J24" t="n">
-        <v>4</v>
-      </c>
-      <c r="K24" t="n">
         <v>342</v>
       </c>
     </row>
@@ -1308,33 +1234,30 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2022</v>
+        <v>263</v>
       </c>
       <c r="C25" t="n">
-        <v>263</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F25" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="H25" t="n">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="I25" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="J25" t="n">
-        <v>2</v>
-      </c>
-      <c r="K25" t="n">
         <v>370</v>
       </c>
     </row>
@@ -1345,31 +1268,28 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2022</v>
+        <v>40</v>
       </c>
       <c r="C26" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D26" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E26" t="n">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F26" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="H26" t="n">
-        <v>64</v>
-      </c>
-      <c r="I26" t="n">
         <v>9</v>
       </c>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="n">
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="n">
         <v>186</v>
       </c>
     </row>
@@ -1380,7 +1300,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2022</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -1395,18 +1315,15 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1417,33 +1334,30 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2021</v>
+        <v>499</v>
       </c>
       <c r="C28" t="n">
-        <v>499</v>
+        <v>304</v>
       </c>
       <c r="D28" t="n">
-        <v>304</v>
+        <v>104</v>
       </c>
       <c r="E28" t="n">
-        <v>104</v>
+        <v>536</v>
       </c>
       <c r="F28" t="n">
-        <v>536</v>
+        <v>19</v>
       </c>
       <c r="G28" t="n">
-        <v>19</v>
+        <v>1601</v>
       </c>
       <c r="H28" t="n">
-        <v>1601</v>
+        <v>65</v>
       </c>
       <c r="I28" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="J28" t="n">
-        <v>32</v>
-      </c>
-      <c r="K28" t="n">
         <v>3160</v>
       </c>
     </row>
@@ -1462,7 +1376,6 @@
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1471,31 +1384,28 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2022</v>
+        <v>14</v>
       </c>
       <c r="C30" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="H30" t="n">
-        <v>256</v>
-      </c>
-      <c r="I30" t="n">
         <v>1</v>
       </c>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="n">
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="n">
         <v>277</v>
       </c>
     </row>
@@ -1510,7 +1420,6 @@
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1527,7 +1436,6 @@
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1544,7 +1452,6 @@
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1561,7 +1468,6 @@
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1578,7 +1484,6 @@
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1595,7 +1500,6 @@
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>